<commit_message>
answered the discussion question (seen at bottom of excel sheets)
</commit_message>
<xml_diff>
--- a/week1day1.xlsx
+++ b/week1day1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julia\Desktop\CSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julia\Desktop\lichjul\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Dividend</t>
   </si>
@@ -39,16 +39,10 @@
     <t>TOTAL PRIMES</t>
   </si>
   <si>
-    <t>Dividend is the number being tested to see if it's prime</t>
+    <t>Response to discussion question:</t>
   </si>
   <si>
-    <t>Not divisible by is a test that evaluates to 1 if the dividend on that row is not divisible by the number in row 2 of the column</t>
-  </si>
-  <si>
-    <t>Is prime evaluates to 1 if the number is prime. This means that there is a "1" in all cells within the the range B to J</t>
-  </si>
-  <si>
-    <t>TOTAL PRIMES counts the number of "1"s in column K</t>
+    <t xml:space="preserve">Although tedious, if I were curious to find the prime numbers between 2 and 100 using excel, I will use what I currently have above and apply it to values (“divided” and “not divided by”) to 100. I will not be able to drag the boxes, because I have to specify which column (“divided”) and row (“divided by”) to use. In other words, I will manually have to go through my code and change the cells  being manipulated. </t>
   </si>
 </sst>
 </file>
@@ -374,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,24 +830,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>